<commit_message>
Update TIL about Java IO, Network Study and R Exam File
</commit_message>
<xml_diff>
--- a/R/R_Workspace/rottentomatoesResult.xlsx
+++ b/R/R_Workspace/rottentomatoesResult.xlsx
@@ -428,34 +428,34 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Toy Story 4 (2019)</t>
+          <t>Knives Out (2019)</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>92%</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Animation, Comedy, Kids &amp; Family, Science Fiction &amp; Fantasy</t>
+          <t>Drama, Mystery &amp; Suspense</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Knives Out (2019)</t>
+          <t>Toy Story 4 (2019)</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>92%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Drama, Mystery &amp; Suspense</t>
+          <t>Animation, Comedy, Kids &amp; Family, Science Fiction &amp; Fantasy</t>
         </is>
       </c>
     </row>
@@ -479,17 +479,17 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>The Farewell (2019)</t>
+          <t>Little Women (2019)</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>87%</t>
+          <t>92%</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Comedy, Drama</t>
+          <t>Drama</t>
         </is>
       </c>
     </row>
@@ -513,17 +513,17 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Little Women (2019)</t>
+          <t>The Farewell (2019)</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>92%</t>
+          <t>87%</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Drama</t>
+          <t>Comedy, Drama</t>
         </is>
       </c>
     </row>
@@ -547,51 +547,51 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Spider-Man: Far From Home (2019)</t>
+          <t>A Beautiful Day in the Neighborhood (2019)</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>92%</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Action &amp; Adventure, Science Fiction &amp; Fantasy</t>
+          <t>Drama</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>If Beale Street Could Talk (2019)</t>
+          <t>Spider-Man: Far From Home (2019)</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>70%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Drama, Romance</t>
+          <t>Action &amp; Adventure, Science Fiction &amp; Fantasy</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>A Beautiful Day in the Neighborhood (2019)</t>
+          <t>If Beale Street Could Talk (2019)</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>92%</t>
+          <t>70%</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Drama</t>
+          <t>Drama, Romance</t>
         </is>
       </c>
     </row>
@@ -637,7 +637,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>83%</t>
+          <t>82%</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -773,7 +773,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>82%</t>
+          <t>81%</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -790,7 +790,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>67%</t>
+          <t>66%</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -994,7 +994,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>86%</t>
+          <t>87%</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1023,68 +1023,68 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Atlantics (2019)</t>
+          <t>Hustlers (2019)</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>83%</t>
+          <t>65%</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Drama, Romance</t>
+          <t>Drama</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Hustlers (2019)</t>
+          <t>Atlantics (2019)</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>65%</t>
+          <t>81%</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Drama</t>
+          <t>Drama, Romance</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>3 Faces (2019)</t>
+          <t>One Child Nation (2019)</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>65%</t>
+          <t>84%</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Art House &amp; International, Drama</t>
+          <t>Documentary</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>One Child Nation (2019)</t>
+          <t>3 Faces (2019)</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>85%</t>
+          <t>67%</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Documentary</t>
+          <t>Art House &amp; International, Drama</t>
         </is>
       </c>
     </row>
@@ -1113,7 +1113,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>90%</t>
+          <t>89%</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -1125,182 +1125,182 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Captain Marvel (2019)</t>
+          <t>Chained for Life (2019)</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>48%</t>
+          <t>63%</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Action &amp; Adventure, Science Fiction &amp; Fantasy</t>
+          <t>Drama</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Midnight Family (2019)</t>
+          <t>Captain Marvel (2019)</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>78%</t>
+          <t>48%</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Documentary</t>
+          <t>Action &amp; Adventure, Science Fiction &amp; Fantasy</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Deadwood: The Movie (2019)</t>
+          <t>Midnight Family (2019)</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>80%</t>
+          <t>78%</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Drama, Western</t>
+          <t>Documentary</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Transit (2019)</t>
+          <t>First Love (Hatsukoi) (2019)</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>63%</t>
+          <t>88%</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Art House &amp; International, Drama</t>
+          <t>Action &amp; Adventure, Drama, Mystery &amp; Suspense</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Midnight Traveler (2019)</t>
+          <t>The Chambermaid (La camarista) (2019)</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>84%</t>
+          <t>60%</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Documentary</t>
+          <t>Art House &amp; International, Drama</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Mickey and the Bear (2019)</t>
+          <t>Deadwood: The Movie (2019)</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>82%</t>
+          <t>79%</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Drama</t>
+          <t>Drama, Western</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>First Love (Hatsukoi) (2019)</t>
+          <t>Midnight Traveler (2019)</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>88%</t>
+          <t>84%</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Action &amp; Adventure, Drama, Mystery &amp; Suspense</t>
+          <t>Documentary</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Tigers Are Not Afraid (Vuelven) (2019)</t>
+          <t>Transit (2019)</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>85%</t>
+          <t>64%</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Art House &amp; International, Drama, Horror, Science Fiction &amp; Fantasy</t>
+          <t>Art House &amp; International, Drama</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Hail Satan? (2019)</t>
+          <t>Mickey and the Bear (2019)</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>85%</t>
+          <t>79%</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Documentary</t>
+          <t>Drama</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Ready or Not (2019)</t>
+          <t>Tigers Are Not Afraid (Vuelven) (2019)</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>78%</t>
+          <t>86%</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Horror, Mystery &amp; Suspense</t>
+          <t>Art House &amp; International, Drama, Horror, Science Fiction &amp; Fantasy</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Toni Morrison: The Pieces I Am (2019)</t>
+          <t>Hail Satan? (2019)</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>96%</t>
+          <t>85%</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -1312,97 +1312,97 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Ad Astra (2019)</t>
+          <t>Toni Morrison: The Pieces I Am (2019)</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>40%</t>
+          <t>96%</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Mystery &amp; Suspense, Science Fiction &amp; Fantasy</t>
+          <t>Documentary</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>The Chambermaid (La camarista) (2019)</t>
+          <t>Ready or Not (2019)</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>61%</t>
+          <t>78%</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Art House &amp; International, Drama</t>
+          <t>Horror, Mystery &amp; Suspense</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Midsommar (2019)</t>
+          <t>Ad Astra (2019)</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>63%</t>
+          <t>40%</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Horror</t>
+          <t>Mystery &amp; Suspense, Science Fiction &amp; Fantasy</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>The Heiresses (Las Herederas) (2019)</t>
+          <t>Midsommar (2019)</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>70%</t>
+          <t>63%</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Drama</t>
+          <t>Horror</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Wild Rose (2019)</t>
+          <t>The Heiresses (Las Herederas) (2019)</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>87%</t>
+          <t>70%</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Comedy, Drama</t>
+          <t>Drama</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Blinded by the Light (2019)</t>
+          <t>Wild Rose (2019)</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>91%</t>
+          <t>87%</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -1414,97 +1414,97 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>63 Up (2019)</t>
+          <t>Blinded by the Light (2019)</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>93%</t>
+          <t>91%</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Documentary</t>
+          <t>Comedy, Drama</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Too Late to Die Young (Tarde para morir joven) (2019)</t>
+          <t>63 Up (2019)</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>45%</t>
+          <t>93%</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Art House &amp; International, Drama</t>
+          <t>Documentary</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Homecoming: A Film by Beyoncé (2019)</t>
+          <t>Too Late to Die Young (Tarde para morir joven) (2019)</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>87%</t>
+          <t>54%</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Documentary, Musical &amp; Performing Arts</t>
+          <t>Art House &amp; International, Drama</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Little Woods (2019)</t>
+          <t>Homecoming: A Film by Beyoncé (2019)</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>53%</t>
+          <t>87%</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Drama</t>
+          <t>Documentary, Musical &amp; Performing Arts</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Rojo (2019)</t>
+          <t>By the Grace of God (Grâce à Dieu) (2019)</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>46%</t>
+          <t>77%</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Drama, Mystery &amp; Suspense</t>
+          <t>Drama</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>By the Grace of God (Grâce à Dieu) (2019)</t>
+          <t>Little Woods (2019)</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>75%</t>
+          <t>54%</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -1516,46 +1516,46 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Gloria Bell (2019)</t>
+          <t>Rojo (2019)</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>44%</t>
+          <t>48%</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Comedy, Romance</t>
+          <t>Drama, Mystery &amp; Suspense</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Chained for Life (2019)</t>
+          <t>Gloria Bell (2019)</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>62%</t>
+          <t>45%</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Drama</t>
+          <t>Comedy, Romance</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Rosie (2019)</t>
+          <t>Dark Waters (2019)</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>76%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -1567,12 +1567,12 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Working Woman (2019)</t>
+          <t>Rosie (2019)</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>100%</t>
+          <t>77%</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -1584,80 +1584,75 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>American Factory (2019)</t>
+          <t>The Mustang (2019)</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>79%</t>
+          <t>74%</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Documentary</t>
+          <t>Drama</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Making Waves: The Art of Cinematic Sound (2019)</t>
-        </is>
-      </c>
-      <c r="B74" t="inlineStr">
-        <is>
-          <t>91%</t>
+          <t>The Garden Left Behind (2019)</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Documentary</t>
+          <t>Drama, Gay &amp; Lesbian</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Fiddler: A Miracle of Miracles (2019)</t>
+          <t>Working Woman (2019)</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>98%</t>
+          <t>100%</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Documentary</t>
+          <t>Drama</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>In Fabric (2019)</t>
+          <t>American Factory (2019)</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>48%</t>
+          <t>79%</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Comedy, Horror</t>
+          <t>Documentary</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Be Natural: The Untold Story of Alice Guy-Blaché (2019)</t>
+          <t>Making Waves: The Art of Cinematic Sound (2019)</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>96%</t>
+          <t>92%</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -1669,17 +1664,17 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>The Mustang (2019)</t>
+          <t>Fiddler: A Miracle of Miracles (2019)</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>74%</t>
+          <t>98%</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Drama</t>
+          <t>Documentary</t>
         </is>
       </c>
     </row>
@@ -1691,7 +1686,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>82%</t>
+          <t>81%</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -1703,128 +1698,133 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>The Garden Left Behind (2019)</t>
+          <t>The Kingmaker (2019)</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>90%</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>Drama, Gay &amp; Lesbian</t>
+          <t>Documentary</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>The Kingmaker (2019)</t>
-        </is>
-      </c>
-      <c r="B81" t="inlineStr">
-        <is>
-          <t>90%</t>
+          <t>I Lost My Body (2019)</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Documentary</t>
+          <t>Animation, Drama, Science Fiction &amp; Fantasy</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Dark Waters (2019)</t>
+          <t>Shadow (2019)</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>80%</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>Drama</t>
+          <t>Action &amp; Adventure, Art House &amp; International, Drama</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Monos (2019)</t>
-        </is>
-      </c>
-      <c r="B83" t="inlineStr">
-        <is>
-          <t>85%</t>
+          <t>Ray &amp; Liz (2019)</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>Drama</t>
+          <t>Art House &amp; International, Drama</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>I Lost My Body (2019)</t>
+          <t>In Fabric (2019)</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>48%</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>Animation, Drama, Science Fiction &amp; Fantasy</t>
+          <t>Comedy, Horror</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Shadow (2019)</t>
+          <t>The Two Popes (2019)</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>79%</t>
+          <t>88%</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>Action &amp; Adventure, Art House &amp; International, Drama</t>
+          <t>Drama</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Ray &amp; Liz (2019)</t>
+          <t>High Flying Bird (2019)</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>42%</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>Art House &amp; International, Drama</t>
+          <t>Drama</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>High Flying Bird (2019)</t>
+          <t>Be Natural: The Untold Story of Alice Guy-Blaché (2019)</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>42%</t>
+          <t>96%</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>Drama</t>
+          <t>Documentary</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Jojo Rabbit (2019)</t>
+          <t>Love, Antosha (2019)</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -1834,19 +1834,19 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>Comedy, Drama</t>
+          <t>Documentary</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>The Two Popes (2019)</t>
+          <t>Monos (2019)</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>88%</t>
+          <t>85%</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
@@ -1858,17 +1858,17 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Love, Antosha (2019)</t>
+          <t>Harpoon (2019)</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>94%</t>
+          <t>62%</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>Documentary</t>
+          <t>Art House &amp; International, Comedy, Horror</t>
         </is>
       </c>
     </row>
@@ -1892,68 +1892,68 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Harpoon (2019)</t>
+          <t>An Elephant Sitting Still (Da xiang xi di er zuo) (2019)</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>59%</t>
+          <t>75%</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>Art House &amp; International, Comedy, Horror</t>
+          <t>Art House &amp; International, Drama</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>An Elephant Sitting Still (Da xiang xi di er zuo) (2019)</t>
+          <t>Luce (2019)</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>74%</t>
+          <t>77%</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>Art House &amp; International, Drama</t>
+          <t>Drama, Mystery &amp; Suspense</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>Luce (2019)</t>
+          <t>Mike Wallace Is Here (2019)</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>77%</t>
+          <t>86%</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>Drama, Mystery &amp; Suspense</t>
+          <t>Documentary</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Mike Wallace Is Here (2019)</t>
+          <t>Jojo Rabbit (2019)</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>86%</t>
+          <t>94%</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>Documentary</t>
+          <t>Comedy, Drama</t>
         </is>
       </c>
     </row>
@@ -1982,7 +1982,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>57%</t>
+          <t>56%</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
@@ -1994,68 +1994,68 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>The Nightingale (2019)</t>
+          <t>Ask Dr. Ruth (2019)</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>73%</t>
+          <t>95%</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>Drama</t>
+          <t>Documentary</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>Ask Dr. Ruth (2019)</t>
+          <t>The Wild Pear Tree (Ahlat agaci) (2019)</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>81%</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>Documentary</t>
+          <t>Drama</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>The Wild Pear Tree (Ahlat agaci) (2019)</t>
+          <t>Citizen K (2019)</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>81%</t>
+          <t>38%</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>Drama</t>
+          <t>Documentary</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>Citizen K (2019)</t>
+          <t>Diane (2019)</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>38%</t>
+          <t>69%</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>Documentary</t>
+          <t>Drama</t>
         </is>
       </c>
     </row>

</xml_diff>